<commit_message>
add bug report, fix clamping
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\GitHub\pathfinder\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\join9\Documents\src\pathfinder\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4858B141-2B25-4741-A792-1A896B5A9F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FA609E-0226-4142-B1E7-2F219CC640D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
+    <workbookView xWindow="5040" yWindow="0" windowWidth="21600" windowHeight="11385" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,73 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+  <si>
+    <t>Bug List</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Reported Date</t>
+  </si>
+  <si>
+    <t>Reported By</t>
+  </si>
+  <si>
+    <t>Severity [P0-P5]</t>
+  </si>
+  <si>
+    <t>Status [open, in-progress, resolved, won't fix]</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Short Desc.</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Steps to reproduce</t>
+  </si>
+  <si>
+    <t>Daniel Lee</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>in-progress</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>When the character collides with a platform wall, it is expected to bounce back in the opposite direction. Instead, the character is currently passing through the wall</t>
+  </si>
+  <si>
+    <t>Upon colliding with the side of a platform, the character should rebound in the opposite direction of the wall</t>
+  </si>
+  <si>
+    <t>The character does not bounce back when colliding with the platform's wall but instead continues through the wall as if no collision occurred.</t>
+  </si>
+  <si>
+    <t>1. Position the character adjacent to a platform wall. 
+2. Move the character towards the platform wall. 
+3. Observe the character's behavior upon collision with the wall.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -45,13 +109,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -63,14 +155,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="강조색1" xfId="1" builtinId="29"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -86,7 +197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -382,12 +493,110 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916EA5C-F684-418E-B4DE-4754B40A2979}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="6" width="23.7109375" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45338</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Open a bug report for character death event
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\join9\Documents\src\pathfinder\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D4B11C-4B75-4A98-844F-112889B7C08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26E11DC-F4A1-44CF-9352-67DD3613F37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Bug List</t>
   </si>
@@ -95,6 +95,25 @@
   </si>
   <si>
     <t>resolved</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>Not yet assigned</t>
+  </si>
+  <si>
+    <t>The character is expected to come to a stop upon death with no animations playing. However, currently, the character continues to move horizontally after death, indicating that horizontal velocity is not being reset.</t>
+  </si>
+  <si>
+    <t>When the character dies (for example, by being hit by a falling boulder), all movement and animations should cease.</t>
+  </si>
+  <si>
+    <t>After the character is hit and the death event is triggered, the character continues to slide horizontally.</t>
+  </si>
+  <si>
+    <t>1. Allow the character to be hit by the boulder to trigger the death sequence.
+2. Observe the character's behavior following the death event.</t>
   </si>
 </sst>
 </file>
@@ -503,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916EA5C-F684-418E-B4DE-4754B40A2979}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,6 +610,38 @@
         <v>17</v>
       </c>
     </row>
+    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5">
+        <v>45338</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed int and float bug in world_system. Added bug-report and test-plan updates
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\join9\Documents\src\pathfinder\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brayd\source\repos\pathfinder\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A41D64-777B-4B91-BF95-D9D2FA82C864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA98375E-DB53-47B9-BBE6-C4078CC245A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Bug List</t>
   </si>
@@ -111,6 +111,82 @@
   </si>
   <si>
     <t>Allan</t>
+  </si>
+  <si>
+    <t>Brayden Shinkawa</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Brayden</t>
+  </si>
+  <si>
+    <t>The character is expected to animate when 
+moving immediately on input, however the 
+movement inputs take an extra second to be noticed. The character will move but not 
+animate for a second after input</t>
+  </si>
+  <si>
+    <t>When the character moves, the 
+character should immediately 
+start its running animation</t>
+  </si>
+  <si>
+    <t>The character takes an extra second after movement input to start its running animation. Releasing another key will also stop running animations</t>
+  </si>
+  <si>
+    <t>1. Move the character
+2. Observe the character not animate its 
+movement in the first second of movement</t>
+  </si>
+  <si>
+    <t>in progress</t>
+  </si>
+  <si>
+    <t>When the character dies and the player 
+continues drawing, the program should 
+reset the scene. Instead, the game crashes</t>
+  </si>
+  <si>
+    <t>When the character dies and the game resets while the player's drawing, the game crashes</t>
+  </si>
+  <si>
+    <t>When the character dies and 
+the game resets while the player's drawing, the game shouldn't crash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Make the character die
+2. While the character is dying, draw on screen
+3. Keep drawing, game will crash
+</t>
+  </si>
+  <si>
+    <t>Joshua Chew</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the character jumps or moves, the movement and jumping should be consistent across multiple machines. However, this is not the case
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When comparing two machines running the game, both players should have similar jump heights and movement speeds
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When comparing two machines running the game, players have differing jump heights and movement speeds
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Run the game on two different cpu setups
+2. Compare jump height and speed of player
+3. If different, problem is still present
+</t>
+  </si>
+  <si>
+    <t>Aaron</t>
   </si>
 </sst>
 </file>
@@ -183,7 +259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -204,10 +280,28 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="강조색1" xfId="1" builtinId="29"/>
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -223,7 +317,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -519,31 +613,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916EA5C-F684-418E-B4DE-4754B40A2979}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16:F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
-    <col min="9" max="9" width="24" customWidth="1"/>
-    <col min="10" max="10" width="39.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="6" width="23.7265625" customWidth="1"/>
+    <col min="7" max="7" width="37.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.453125" customWidth="1"/>
+    <col min="9" max="9" width="27.6328125" customWidth="1"/>
+    <col min="10" max="10" width="39.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -575,7 +669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -607,7 +701,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>2</v>
       </c>
@@ -639,7 +733,267 @@
         <v>22</v>
       </c>
     </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="10">
+        <v>3</v>
+      </c>
+      <c r="B6" s="11">
+        <v>45375</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="10">
+        <v>4</v>
+      </c>
+      <c r="B11" s="11">
+        <v>45375</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="10">
+        <v>5</v>
+      </c>
+      <c r="B16" s="11">
+        <v>45375</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+    </row>
   </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="F16:F19"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F11:F15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="E16:E19"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated bug reports and test plan
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brayd\source\repos\pathfinder\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA98375E-DB53-47B9-BBE6-C4078CC245A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66E3A53-DB57-4118-BBFC-110A010741A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
   <si>
     <t>Bug List</t>
   </si>
@@ -187,6 +187,66 @@
   </si>
   <si>
     <t>Aaron</t>
+  </si>
+  <si>
+    <t>P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the character moves right and adds a short left movement, the player will continue to slide left even after the player stops pressing key inputs
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the character presses the A or D keys for moving left and right, they should move in their respective directions. If no keys are pressed, the player shouldn't move
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Player continue moves without deaccelerating even when no input keys are pressed
+</t>
+  </si>
+  <si>
+    <t>1. Make the character move right
+2. Quickly press the left move button
+3. Player should start sliding left without deaccelerating</t>
+  </si>
+  <si>
+    <t>Anyone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the player respawns at a checkpoint flag, the checkpoint sound continues to play
+</t>
+  </si>
+  <si>
+    <t>Aaron Zhang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the player respawns at the checkpoint flag, no checkpoint sound should occur
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the player respawns at the checkpoint flag, the checkpoint sound repeats instead of staying silent
+</t>
+  </si>
+  <si>
+    <t>1. Get player to hit a checkpoint (sound should play)
+2. Get player to respawn at checkpoint by pressing L
+3. Checkpoint sound will continue to repeat as long as the player stands on the checkpoint</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
+    <t>When the player respawns and is falling down, they will be stuck in the running loop animation, even when not moving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When the player respawns, they should be in the neutral player texture frame
+</t>
+  </si>
+  <si>
+    <t>When the player respawns, they are stuck in the running loop animation, even when not moving</t>
+  </si>
+  <si>
+    <t>1. Get player to respawn
+2. player randomly respawns in run animation</t>
   </si>
 </sst>
 </file>
@@ -259,7 +319,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -283,17 +343,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -613,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916EA5C-F684-418E-B4DE-4754B40A2979}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:F19"/>
+    <sheetView tabSelected="1" topLeftCell="B20" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -734,232 +809,328 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="10">
+      <c r="A6" s="16">
         <v>3</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="17">
         <v>45375</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="13" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="10">
+      <c r="A11" s="16">
         <v>4</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="17">
         <v>45375</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="16"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A16" s="16">
+        <v>5</v>
+      </c>
+      <c r="B16" s="17">
+        <v>45375</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A17" s="16"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A19" s="16"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+    </row>
+    <row r="20" spans="1:10" ht="116" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>6</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45375</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="10">
-        <v>5</v>
-      </c>
-      <c r="B16" s="11">
+      <c r="F20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5">
         <v>45375</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="10"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="10"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+      <c r="D21" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
+        <v>8</v>
+      </c>
+      <c r="B22" s="5">
+        <v>45375</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>

<commit_message>
esolved checkpoint sound bug
</commit_message>
<xml_diff>
--- a/doc/bug-report.xlsx
+++ b/doc/bug-report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brayd\source\repos\pathfinder\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4629DB9A-B100-48BC-BDBD-844AA4F98754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB5905D-9135-49C5-9AF8-C9A613F978CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{2EEE4158-1D5F-475F-A63E-5C076E84441D}"/>
   </bookViews>
@@ -362,13 +362,13 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -690,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D916EA5C-F684-418E-B4DE-4754B40A2979}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -809,22 +809,22 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="16">
+      <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="16">
         <v>45375</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="17" t="s">
         <v>26</v>
       </c>
       <c r="G6" s="13" t="s">
@@ -841,70 +841,70 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="16"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
       <c r="E7" s="18"/>
-      <c r="F7" s="15"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
       <c r="E8" s="18"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="15"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="16"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
       <c r="E10" s="18"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="16">
+      <c r="A11" s="15">
         <v>4</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>45375</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="17" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="13" t="s">
@@ -921,70 +921,70 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="16"/>
-      <c r="B12" s="16"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
       <c r="E12" s="18"/>
-      <c r="F12" s="15"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="16"/>
-      <c r="B13" s="16"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="A13" s="15"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
       <c r="E13" s="18"/>
-      <c r="F13" s="15"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
       <c r="E15" s="18"/>
-      <c r="F15" s="15"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="16">
+      <c r="A16" s="15">
         <v>5</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="16">
         <v>45375</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="17" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="17" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="13" t="s">
@@ -1001,36 +1001,36 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="16"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A19" s="16"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
@@ -1082,10 +1082,10 @@
         <v>43</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>49</v>
@@ -1134,16 +1134,14 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="A6:A10"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="D6:D10"/>
-    <mergeCell ref="E6:E10"/>
-    <mergeCell ref="F6:F10"/>
-    <mergeCell ref="G6:G10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="G16:G19"/>
+    <mergeCell ref="H16:H19"/>
+    <mergeCell ref="I16:I19"/>
+    <mergeCell ref="J16:J19"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H15"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="J11:J15"/>
     <mergeCell ref="F16:F19"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="B11:B15"/>
@@ -1156,14 +1154,16 @@
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="D16:D19"/>
     <mergeCell ref="E16:E19"/>
-    <mergeCell ref="G16:G19"/>
-    <mergeCell ref="H16:H19"/>
-    <mergeCell ref="I16:I19"/>
-    <mergeCell ref="J16:J19"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="H11:H15"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="J11:J15"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="D6:D10"/>
+    <mergeCell ref="E6:E10"/>
+    <mergeCell ref="F6:F10"/>
+    <mergeCell ref="G6:G10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>